<commit_message>
WIP: Isotonic method approved (need the pava case) / restructed the Compute_AgeS_D function to be used / Added the Independance model for Jags
</commit_message>
<xml_diff>
--- a/R/DataManipulation/All_Qz_Grains_BayLum_doses.xlsx
+++ b/R/DataManipulation/All_Qz_Grains_BayLum_doses.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\esellwood\Documents\3. CPJB OSL\2. Analysis\2. Analysis and BayLum Modelling\Data for Imene\Individual Var\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniren1-my.sharepoint.com/personal/elaine_sellwood_univ-rennes_fr/Documents/Post Doc-PR048038/3. CPJB OSL/Imène Models/Data for Imene/20250624 Palaeodose Computation results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FCAF0C-DD87-4272-943D-D495D3989E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{86FCAF0C-DD87-4272-943D-D495D3989E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E785199F-8889-48A7-8B32-166A533D4A09}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-2565" windowWidth="25440" windowHeight="15270" xr2:uid="{80AF7415-E759-490E-8D0C-585C5C5F61D6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{80AF7415-E759-490E-8D0C-585C5C5F61D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
-    <sheet name="Central doses No Strat" sheetId="1" r:id="rId2"/>
-    <sheet name="Central doses Strat and Cov" sheetId="2" r:id="rId3"/>
+    <sheet name="General stats" sheetId="7" r:id="rId2"/>
+    <sheet name="Dose estimates" sheetId="1" r:id="rId3"/>
     <sheet name="Dose rate" sheetId="3" r:id="rId4"/>
-    <sheet name="CoVar Theta Matrix" sheetId="4" r:id="rId5"/>
+    <sheet name="CoVar Theta Matrix" sheetId="8" r:id="rId5"/>
     <sheet name="Strat Matrix" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="113">
   <si>
     <t>lower bound at 95%</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Convergencies: uppers confidence interval</t>
   </si>
   <si>
-    <t xml:space="preserve">Layer </t>
-  </si>
-  <si>
     <t>CPJB_L7</t>
   </si>
   <si>
@@ -194,27 +191,12 @@
     <t>V15</t>
   </si>
   <si>
-    <t>Uncertainty</t>
-  </si>
-  <si>
-    <t>Central dose No strat</t>
-  </si>
-  <si>
-    <t>Central dises Strat and Cov</t>
-  </si>
-  <si>
     <t>Sheet</t>
   </si>
   <si>
     <t>Contents</t>
   </si>
   <si>
-    <t>Central doses and confidence intervals from BayLum, for all quartz grains. No stratigraphic constraints or shared uncertanties.</t>
-  </si>
-  <si>
-    <t>Central doses and confidence intervals from BayLum, for all quartz grains. WITH stratigraphic constraints and shared uncertanties.</t>
-  </si>
-  <si>
     <t>Dose rate</t>
   </si>
   <si>
@@ -240,14 +222,171 @@
   </si>
   <si>
     <t>Notes:</t>
+  </si>
+  <si>
+    <t>Depth mm</t>
+  </si>
+  <si>
+    <t>D_CPJB_L7</t>
+  </si>
+  <si>
+    <t>D_CPJB_L8</t>
+  </si>
+  <si>
+    <t>D_CPJB_L9</t>
+  </si>
+  <si>
+    <t>D_CPJB_L10</t>
+  </si>
+  <si>
+    <t>D_CPJB_L11</t>
+  </si>
+  <si>
+    <t>D_CPJB_L12</t>
+  </si>
+  <si>
+    <t>D_CPJB_L13</t>
+  </si>
+  <si>
+    <t>D_CPJB_L14</t>
+  </si>
+  <si>
+    <t>D_CPJB_L15</t>
+  </si>
+  <si>
+    <t>D_CPJB_L16</t>
+  </si>
+  <si>
+    <t>D_CPJB_L17</t>
+  </si>
+  <si>
+    <t>D_CPJB_L18</t>
+  </si>
+  <si>
+    <t>D_CPJB_L19</t>
+  </si>
+  <si>
+    <t>D_CPJB_L20</t>
+  </si>
+  <si>
+    <t>D_CPJB_L21</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L7</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L8</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L9</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L10</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L11</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L12</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L13</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L14</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L15</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L16</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L17</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L18</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L19</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L20</t>
+  </si>
+  <si>
+    <t>sD_CPJB_L21</t>
+  </si>
+  <si>
+    <t>Layer</t>
+  </si>
+  <si>
+    <t>Depth (mm)</t>
+  </si>
+  <si>
+    <t>OD</t>
+  </si>
+  <si>
+    <t>Mean De Gy</t>
+  </si>
+  <si>
+    <t>StdEr Gy</t>
+  </si>
+  <si>
+    <t>De err</t>
+  </si>
+  <si>
+    <t>OD_err</t>
+  </si>
+  <si>
+    <t>CAM De</t>
+  </si>
+  <si>
+    <t>Dose estimates</t>
+  </si>
+  <si>
+    <t>R Code:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de_est = Palaeodose_Computation(DATA, SampleNames=Names, Nb_sample=Nb_sample, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               BinPerSample = rep(2,Nb_sample), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               SavePdf = TRUE, SaveEstimates = TRUE, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               LIN_fit = TRUE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               Origin_fit = FALSE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               distribution = c("lognormal_A"),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               Iter = 80000,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               t = 5,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               n.chains = 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Results from running Palaeodose_Computation, with both results for D and sD parameters, alongside sample depth. </t>
+  </si>
+  <si>
+    <t>Parameter and Layer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -298,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -306,6 +445,7 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,75 +760,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533D7F98-DD1C-48F5-BCD7-95646A84A540}">
-  <dimension ref="B3:F14"/>
+  <dimension ref="B3:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>64</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -698,492 +883,432 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BCEDA09-C07F-46D9-B572-DC73A31E7828}">
-  <dimension ref="A1:I16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E29FF8B-8C6F-47C6-801D-ADD67947C08B}">
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="11" max="11" width="15.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" s="7">
+        <v>20.355560000000001</v>
+      </c>
+      <c r="C2">
+        <v>49.561543452381002</v>
+      </c>
+      <c r="D2">
+        <v>2.7104347769279098</v>
+      </c>
+      <c r="E2">
+        <v>41.237805393248202</v>
+      </c>
+      <c r="F2">
+        <v>1.5113254102090601</v>
+      </c>
+      <c r="G2">
+        <v>17.893181954916599</v>
+      </c>
+      <c r="H2">
+        <v>1.1319651474997201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>69.991</v>
-      </c>
-      <c r="C2">
-        <v>76.102999999999994</v>
-      </c>
-      <c r="D2">
-        <v>84.813000000000002</v>
-      </c>
-      <c r="E2">
-        <v>91.367000000000004</v>
-      </c>
-      <c r="F2">
-        <v>100.59099999999999</v>
-      </c>
-      <c r="G2">
-        <f>(F2-B2)/2</f>
-        <v>15.299999999999997</v>
-      </c>
-      <c r="H2">
-        <v>1.2549999999999999</v>
-      </c>
-      <c r="I2">
-        <v>1.7090000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3" s="7">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="C3">
+        <v>35.277165170068002</v>
+      </c>
+      <c r="D3">
+        <v>1.98313703736433</v>
+      </c>
+      <c r="E3">
+        <v>39.8616826171694</v>
+      </c>
+      <c r="F3">
+        <v>1.1196536450021699</v>
+      </c>
+      <c r="G3">
+        <v>14.2186483069475</v>
+      </c>
+      <c r="H3">
+        <v>0.84317611605522902</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
-        <v>61.454999999999998</v>
-      </c>
-      <c r="C3">
-        <v>64.555999999999997</v>
-      </c>
-      <c r="D3">
-        <v>68.894000000000005</v>
-      </c>
-      <c r="E3">
-        <v>72.266000000000005</v>
-      </c>
-      <c r="F3">
-        <v>76.683000000000007</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G16" si="0">(F3-B3)/2</f>
-        <v>7.6140000000000043</v>
-      </c>
-      <c r="H3">
-        <v>1.004</v>
-      </c>
-      <c r="I3">
-        <v>1.0049999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B4" s="7">
+        <v>17.271429999999999</v>
+      </c>
+      <c r="C4">
+        <v>49.540594433962298</v>
+      </c>
+      <c r="D4">
+        <v>2.1028740318195198</v>
+      </c>
+      <c r="E4">
+        <v>43.219151705128198</v>
+      </c>
+      <c r="F4">
+        <v>1.3903677572964299</v>
+      </c>
+      <c r="G4">
+        <v>19.001006191507901</v>
+      </c>
+      <c r="H4">
+        <v>1.0340239205952499</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
-        <v>65.16</v>
-      </c>
-      <c r="C4">
-        <v>68.186000000000007</v>
-      </c>
-      <c r="D4">
-        <v>72.186999999999998</v>
-      </c>
-      <c r="E4">
-        <v>75.381</v>
-      </c>
-      <c r="F4">
-        <v>79.456000000000003</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>7.1480000000000032</v>
-      </c>
-      <c r="H4">
-        <v>1.0029999999999999</v>
-      </c>
-      <c r="I4">
-        <v>1.01</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5" s="7">
+        <v>16.533329999999999</v>
+      </c>
+      <c r="C5">
+        <v>84.038780113636406</v>
+      </c>
+      <c r="D5">
+        <v>3.6523817505667302</v>
+      </c>
+      <c r="E5">
+        <v>69.9307818466783</v>
+      </c>
+      <c r="F5">
+        <v>2.59058299144445</v>
+      </c>
+      <c r="G5">
+        <v>29.987491601717199</v>
+      </c>
+      <c r="H5">
+        <v>1.9671361110721499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
-        <v>97.870999999999995</v>
-      </c>
-      <c r="C5">
-        <v>100.78400000000001</v>
-      </c>
-      <c r="D5">
-        <v>104.142</v>
-      </c>
-      <c r="E5">
-        <v>107.066</v>
-      </c>
-      <c r="F5">
-        <v>110.541</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>6.3350000000000009</v>
-      </c>
-      <c r="H5">
-        <v>1.0029999999999999</v>
-      </c>
-      <c r="I5">
-        <v>1.0069999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B6" s="7">
+        <v>14.16667</v>
+      </c>
+      <c r="C6">
+        <v>80.842016132596697</v>
+      </c>
+      <c r="D6">
+        <v>3.2144867798986798</v>
+      </c>
+      <c r="E6">
+        <v>70.971846943202607</v>
+      </c>
+      <c r="F6">
+        <v>2.01893082088014</v>
+      </c>
+      <c r="G6">
+        <v>22.9850904476612</v>
+      </c>
+      <c r="H6">
+        <v>1.5645105262029499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B6">
-        <v>95.462000000000003</v>
-      </c>
-      <c r="C6">
-        <v>97.974999999999994</v>
-      </c>
-      <c r="D6">
-        <v>101.33499999999999</v>
-      </c>
-      <c r="E6">
-        <v>104.101</v>
-      </c>
-      <c r="F6">
-        <v>107.506</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>6.0219999999999985</v>
-      </c>
-      <c r="H6">
-        <v>1.01</v>
-      </c>
-      <c r="I6">
-        <v>1.0349999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B7" s="7">
+        <v>13.377780000000001</v>
+      </c>
+      <c r="C7">
+        <v>81.464782371134007</v>
+      </c>
+      <c r="D7">
+        <v>3.0283097889760602</v>
+      </c>
+      <c r="E7">
+        <v>74.341906973984194</v>
+      </c>
+      <c r="F7">
+        <v>2.1335108157073202</v>
+      </c>
+      <c r="G7">
+        <v>25.728645198859301</v>
+      </c>
+      <c r="H7">
+        <v>1.65179315153243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B7">
-        <v>107.526</v>
-      </c>
-      <c r="C7">
-        <v>111.116</v>
-      </c>
-      <c r="D7">
-        <v>115.58799999999999</v>
-      </c>
-      <c r="E7">
-        <v>119.446</v>
-      </c>
-      <c r="F7">
-        <v>123.917</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>8.1955000000000027</v>
-      </c>
-      <c r="H7">
-        <v>1.0189999999999999</v>
-      </c>
-      <c r="I7">
-        <v>1.06</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B8" s="7">
+        <v>12.377780000000001</v>
+      </c>
+      <c r="C8">
+        <v>86.544521538461495</v>
+      </c>
+      <c r="D8">
+        <v>3.3425131589850201</v>
+      </c>
+      <c r="E8">
+        <v>75.267192801933504</v>
+      </c>
+      <c r="F8">
+        <v>2.7758228762819401</v>
+      </c>
+      <c r="G8">
+        <v>34.947521110795499</v>
+      </c>
+      <c r="H8">
+        <v>2.0913616615205499</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B8">
-        <v>127.887</v>
-      </c>
-      <c r="C8">
-        <v>134.77500000000001</v>
-      </c>
-      <c r="D8">
-        <v>149.22200000000001</v>
-      </c>
-      <c r="E8">
-        <v>157.12899999999999</v>
-      </c>
-      <c r="F8">
-        <v>176.459</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>24.286000000000001</v>
-      </c>
-      <c r="H8">
-        <v>1.294</v>
-      </c>
-      <c r="I8">
-        <v>1.796</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B9" s="7">
+        <v>10.977779999999999</v>
+      </c>
+      <c r="C9">
+        <v>91.838232830188701</v>
+      </c>
+      <c r="D9">
+        <v>4.1695468727777403</v>
+      </c>
+      <c r="E9">
+        <v>80.426342068341</v>
+      </c>
+      <c r="F9">
+        <v>2.5887943598805001</v>
+      </c>
+      <c r="G9">
+        <v>27.986320830419899</v>
+      </c>
+      <c r="H9">
+        <v>2.01379678783589</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B9">
-        <v>120.523</v>
-      </c>
-      <c r="C9">
-        <v>126.065</v>
-      </c>
-      <c r="D9">
-        <v>133.447</v>
-      </c>
-      <c r="E9">
-        <v>139.31100000000001</v>
-      </c>
-      <c r="F9">
-        <v>146.94399999999999</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>13.210499999999996</v>
-      </c>
-      <c r="H9">
-        <v>1.028</v>
-      </c>
-      <c r="I9">
-        <v>1.0860000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B10" s="7">
+        <v>9.5444400000000016</v>
+      </c>
+      <c r="C10">
+        <v>82.455403571428604</v>
+      </c>
+      <c r="D10">
+        <v>3.2428710590249201</v>
+      </c>
+      <c r="E10">
+        <v>75.032029571629707</v>
+      </c>
+      <c r="F10">
+        <v>2.7856438462103399</v>
+      </c>
+      <c r="G10">
+        <v>28.0541607556993</v>
+      </c>
+      <c r="H10">
+        <v>2.1536447096290798</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B10">
-        <v>99.132000000000005</v>
-      </c>
-      <c r="C10">
-        <v>102.43300000000001</v>
-      </c>
-      <c r="D10">
-        <v>106.88800000000001</v>
-      </c>
-      <c r="E10">
-        <v>110.517</v>
-      </c>
-      <c r="F10">
-        <v>115.504</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>8.1859999999999999</v>
-      </c>
-      <c r="H10">
-        <v>1.0129999999999999</v>
-      </c>
-      <c r="I10">
-        <v>1.044</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B11" s="7">
+        <v>7.4555600000000002</v>
+      </c>
+      <c r="C11">
+        <v>82.260733061224499</v>
+      </c>
+      <c r="D11">
+        <v>2.5631466188744398</v>
+      </c>
+      <c r="E11">
+        <v>74.410044329428203</v>
+      </c>
+      <c r="F11">
+        <v>1.9925849265859401</v>
+      </c>
+      <c r="G11">
+        <v>27.1614079016964</v>
+      </c>
+      <c r="H11">
+        <v>1.5282814064925201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B11">
-        <v>99.855000000000004</v>
-      </c>
-      <c r="C11">
-        <v>102.989</v>
-      </c>
-      <c r="D11">
-        <v>106.9</v>
-      </c>
-      <c r="E11">
-        <v>110.238</v>
-      </c>
-      <c r="F11">
-        <v>114.232</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>7.1884999999999977</v>
-      </c>
-      <c r="H11">
-        <v>1.002</v>
-      </c>
-      <c r="I11">
-        <v>1.0029999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B12" s="7">
+        <v>6.0888899999999992</v>
+      </c>
+      <c r="C12">
+        <v>89.691951860465096</v>
+      </c>
+      <c r="D12">
+        <v>3.3265483943985501</v>
+      </c>
+      <c r="E12">
+        <v>78.193779693978001</v>
+      </c>
+      <c r="F12">
+        <v>2.36981970987476</v>
+      </c>
+      <c r="G12">
+        <v>25.304583245975099</v>
+      </c>
+      <c r="H12">
+        <v>1.89750011037272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B12">
-        <v>113.44199999999999</v>
-      </c>
-      <c r="C12">
-        <v>118.01</v>
-      </c>
-      <c r="D12">
-        <v>123.807</v>
-      </c>
-      <c r="E12">
-        <v>128.38900000000001</v>
-      </c>
-      <c r="F12">
-        <v>134.32900000000001</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>10.443500000000007</v>
-      </c>
-      <c r="H12">
-        <v>1.032</v>
-      </c>
-      <c r="I12">
-        <v>1.1020000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="B13" s="7">
+        <v>5.0374999999999996</v>
+      </c>
+      <c r="C13">
+        <v>104.618674569536</v>
+      </c>
+      <c r="D13">
+        <v>5.2555531200178498</v>
+      </c>
+      <c r="E13">
+        <v>87.227845774688404</v>
+      </c>
+      <c r="F13">
+        <v>3.2308649615610698</v>
+      </c>
+      <c r="G13">
+        <v>33.657671005264802</v>
+      </c>
+      <c r="H13">
+        <v>2.4628654600527802</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B13">
-        <v>130.50399999999999</v>
-      </c>
-      <c r="C13">
-        <v>136.88</v>
-      </c>
-      <c r="D13">
-        <v>145.072</v>
-      </c>
-      <c r="E13">
-        <v>151.51599999999999</v>
-      </c>
-      <c r="F13">
-        <v>160.965</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>15.230500000000006</v>
-      </c>
-      <c r="H13">
-        <v>1.004</v>
-      </c>
-      <c r="I13">
-        <v>1.0149999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="B14" s="7">
+        <v>3.5777800000000006</v>
+      </c>
+      <c r="C14">
+        <v>84.838674037267097</v>
+      </c>
+      <c r="D14">
+        <v>2.9121259543898499</v>
+      </c>
+      <c r="E14">
+        <v>76.409046047432597</v>
+      </c>
+      <c r="F14">
+        <v>2.50275449579456</v>
+      </c>
+      <c r="G14">
+        <v>25.2803361924149</v>
+      </c>
+      <c r="H14">
+        <v>2.03157748938251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B14">
-        <v>106.74</v>
-      </c>
-      <c r="C14">
-        <v>110.569</v>
-      </c>
-      <c r="D14">
-        <v>115.846</v>
-      </c>
-      <c r="E14">
-        <v>119.92400000000001</v>
-      </c>
-      <c r="F14">
-        <v>125.16200000000001</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>9.2110000000000056</v>
-      </c>
-      <c r="H14">
-        <v>1.042</v>
-      </c>
-      <c r="I14">
-        <v>1.133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B15" s="7">
+        <v>2.9666700000000006</v>
+      </c>
+      <c r="C15">
+        <v>77.627659342105304</v>
+      </c>
+      <c r="D15">
+        <v>3.3578307999704</v>
+      </c>
+      <c r="E15">
+        <v>64.445624455815803</v>
+      </c>
+      <c r="F15">
+        <v>3.2378072485252001</v>
+      </c>
+      <c r="G15">
+        <v>34.713374810361699</v>
+      </c>
+      <c r="H15">
+        <v>2.4679589861108702</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B15">
-        <v>95.43</v>
-      </c>
-      <c r="C15">
-        <v>99.320999999999998</v>
-      </c>
-      <c r="D15">
-        <v>104.102</v>
-      </c>
-      <c r="E15">
-        <v>108.122</v>
-      </c>
-      <c r="F15">
-        <v>112.917</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>8.7434999999999974</v>
-      </c>
-      <c r="H15">
-        <v>1.0329999999999999</v>
-      </c>
-      <c r="I15">
-        <v>1.1040000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16">
-        <v>77.314999999999998</v>
+      <c r="B16" s="7">
+        <v>2.1888900000000007</v>
       </c>
       <c r="C16">
-        <v>79.664000000000001</v>
+        <v>62.365977793103397</v>
       </c>
       <c r="D16">
-        <v>82.445999999999998</v>
+        <v>2.3734755349629801</v>
       </c>
       <c r="E16">
-        <v>85.055999999999997</v>
+        <v>57.505628161045799</v>
       </c>
       <c r="F16">
-        <v>87.89</v>
+        <v>1.9801049026766899</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
-        <v>5.2875000000000014</v>
+        <v>19.604470053039002</v>
       </c>
       <c r="H16">
-        <v>1.006</v>
-      </c>
-      <c r="I16">
-        <v>1.022</v>
+        <v>1.5702029713052501</v>
       </c>
     </row>
   </sheetData>
@@ -1192,36 +1317,43 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80EA0D23-7AAC-4AA6-86E0-41F2037C1DA7}">
-  <dimension ref="A1:I16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BCEDA09-C07F-46D9-B572-DC73A31E7828}">
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1231,454 +1363,919 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>63.027000000000001</v>
+      <c r="A2" s="7">
+        <v>20.355560000000001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
       </c>
       <c r="C2">
-        <v>68.248999999999995</v>
+        <v>57</v>
       </c>
       <c r="D2">
-        <v>72.747</v>
+        <v>62</v>
       </c>
       <c r="E2">
-        <v>77.113</v>
+        <v>69.376999999999995</v>
       </c>
       <c r="F2">
-        <v>82.540999999999997</v>
+        <v>75</v>
       </c>
       <c r="G2">
-        <f>(F2-B2)/2</f>
-        <v>9.7569999999999979</v>
+        <v>84</v>
       </c>
       <c r="H2">
-        <v>1.339</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>1.893</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>63.960999999999999</v>
+      <c r="A3" s="7">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
       </c>
       <c r="C3">
-        <v>66.97</v>
+        <v>50</v>
       </c>
       <c r="D3">
-        <v>71.260999999999996</v>
+        <v>53</v>
       </c>
       <c r="E3">
-        <v>74.834000000000003</v>
+        <v>57.408999999999999</v>
       </c>
       <c r="F3">
-        <v>78.847999999999999</v>
+        <v>61</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G16" si="0">(F3-B3)/2</f>
-        <v>7.4435000000000002</v>
+        <v>66</v>
       </c>
       <c r="H3">
-        <v>1.5569999999999999</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>2.4239999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>67.375</v>
+      <c r="A4" s="7">
+        <v>17.271429999999999</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
       </c>
       <c r="C4">
-        <v>70.548000000000002</v>
+        <v>53</v>
       </c>
       <c r="D4">
-        <v>75.236000000000004</v>
+        <v>57</v>
       </c>
       <c r="E4">
-        <v>78.778999999999996</v>
+        <v>60.401000000000003</v>
       </c>
       <c r="F4">
-        <v>83.668000000000006</v>
+        <v>64</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
-        <v>8.1465000000000032</v>
+        <v>68</v>
       </c>
       <c r="H4">
-        <v>1.4079999999999999</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>2.0550000000000002</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>95.578999999999994</v>
+      <c r="A5" s="7">
+        <v>16.533329999999999</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
       </c>
       <c r="C5">
-        <v>98.936000000000007</v>
+        <v>83</v>
       </c>
       <c r="D5">
-        <v>102.83799999999999</v>
+        <v>87</v>
       </c>
       <c r="E5">
-        <v>105.494</v>
+        <v>92.007999999999996</v>
       </c>
       <c r="F5">
-        <v>110.467</v>
+        <v>96</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
-        <v>7.4440000000000026</v>
+        <v>101</v>
       </c>
       <c r="H5">
-        <v>1.0289999999999999</v>
+        <v>1.01</v>
       </c>
       <c r="I5">
-        <v>1.0509999999999999</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>96.471000000000004</v>
+      <c r="A6" s="7">
+        <v>14.16667</v>
+      </c>
+      <c r="B6" t="s">
+        <v>66</v>
       </c>
       <c r="C6">
-        <v>99.04</v>
+        <v>78</v>
       </c>
       <c r="D6">
-        <v>102.301</v>
+        <v>81</v>
       </c>
       <c r="E6">
-        <v>105.047</v>
+        <v>84.054000000000002</v>
       </c>
       <c r="F6">
-        <v>108.267</v>
+        <v>87</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
-        <v>5.8979999999999961</v>
+        <v>91</v>
       </c>
       <c r="H6">
-        <v>1.0189999999999999</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>1.0649999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>106.233</v>
+      <c r="A7" s="7">
+        <v>13.377780000000001</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
       </c>
       <c r="C7">
-        <v>110.38500000000001</v>
+        <v>91</v>
       </c>
       <c r="D7">
-        <v>114.779</v>
+        <v>95</v>
       </c>
       <c r="E7">
-        <v>117.428</v>
+        <v>100.44799999999999</v>
       </c>
       <c r="F7">
-        <v>122.47199999999999</v>
+        <v>105</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
-        <v>8.1194999999999951</v>
+        <v>111</v>
       </c>
       <c r="H7">
-        <v>1.141</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>1.413</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>114.45699999999999</v>
+      <c r="A8" s="7">
+        <v>12.377780000000001</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
       </c>
       <c r="C8">
-        <v>117.273</v>
+        <v>109</v>
       </c>
       <c r="D8">
-        <v>129.78700000000001</v>
+        <v>115</v>
       </c>
       <c r="E8">
-        <v>130.06800000000001</v>
+        <v>124.879</v>
       </c>
       <c r="F8">
-        <v>160.27099999999999</v>
+        <v>132</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
-        <v>22.906999999999996</v>
+        <v>142</v>
       </c>
       <c r="H8">
-        <v>1.244</v>
+        <v>1.01</v>
       </c>
       <c r="I8">
-        <v>1.681</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>114.744</v>
+      <c r="A9" s="7">
+        <v>10.977779999999999</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
       </c>
       <c r="C9">
-        <v>118.22199999999999</v>
+        <v>106</v>
       </c>
       <c r="D9">
-        <v>130.797</v>
+        <v>113</v>
       </c>
       <c r="E9">
-        <v>130.36799999999999</v>
+        <v>122.349</v>
       </c>
       <c r="F9">
-        <v>178.327</v>
+        <v>130</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
-        <v>31.791499999999999</v>
+        <v>138</v>
       </c>
       <c r="H9">
-        <v>1.0780000000000001</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>1.2490000000000001</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="7">
+        <v>9.5444400000000016</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10">
+        <v>91</v>
+      </c>
+      <c r="D10">
+        <v>96</v>
+      </c>
+      <c r="E10">
+        <v>103.565</v>
+      </c>
+      <c r="F10">
+        <v>109</v>
+      </c>
+      <c r="G10">
+        <v>117</v>
+      </c>
+      <c r="H10">
+        <v>1.02</v>
+      </c>
+      <c r="I10">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
+        <v>7.4555600000000002</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11">
+        <v>87</v>
+      </c>
+      <c r="D11">
+        <v>89</v>
+      </c>
+      <c r="E11">
+        <v>92.941000000000003</v>
+      </c>
+      <c r="F11">
+        <v>96</v>
+      </c>
+      <c r="G11">
+        <v>101</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="7">
+        <v>6.0888899999999992</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12">
+        <v>108</v>
+      </c>
+      <c r="D12">
+        <v>112</v>
+      </c>
+      <c r="E12">
+        <v>119.49299999999999</v>
+      </c>
+      <c r="F12">
+        <v>125</v>
+      </c>
+      <c r="G12">
+        <v>133</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="7">
+        <v>5.0374999999999996</v>
+      </c>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13">
+        <v>125</v>
+      </c>
+      <c r="D13">
+        <v>132</v>
+      </c>
+      <c r="E13">
+        <v>140.67699999999999</v>
+      </c>
+      <c r="F13">
+        <v>148</v>
+      </c>
+      <c r="G13">
+        <v>158</v>
+      </c>
+      <c r="H13">
+        <v>1.01</v>
+      </c>
+      <c r="I13">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="7">
+        <v>3.5777800000000006</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14">
+        <v>91</v>
+      </c>
+      <c r="D14">
+        <v>95</v>
+      </c>
+      <c r="E14">
+        <v>100.652</v>
+      </c>
+      <c r="F14">
+        <v>106</v>
+      </c>
+      <c r="G14">
+        <v>111</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="7">
+        <v>2.9666700000000006</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15">
+        <v>82</v>
+      </c>
+      <c r="D15">
+        <v>87</v>
+      </c>
+      <c r="E15">
+        <v>92.75</v>
+      </c>
+      <c r="F15">
+        <v>97</v>
+      </c>
+      <c r="G15">
+        <v>104</v>
+      </c>
+      <c r="H15">
+        <v>1.01</v>
+      </c>
+      <c r="I15">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="7">
+        <v>2.1888900000000007</v>
+      </c>
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16">
+        <v>63</v>
+      </c>
+      <c r="D16">
+        <v>65</v>
+      </c>
+      <c r="E16">
+        <v>67.850999999999999</v>
+      </c>
+      <c r="F16">
+        <v>71</v>
+      </c>
+      <c r="G16">
+        <v>74</v>
+      </c>
+      <c r="H16">
+        <v>1.02</v>
+      </c>
+      <c r="I16">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="7">
+        <v>20.355560000000001</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17">
+        <v>42</v>
+      </c>
+      <c r="D17">
+        <v>48</v>
+      </c>
+      <c r="E17">
+        <v>62.991999999999997</v>
+      </c>
+      <c r="F17">
+        <v>71</v>
+      </c>
+      <c r="G17">
+        <v>88</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="7">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="B18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18">
+        <v>27</v>
+      </c>
+      <c r="D18">
+        <v>31</v>
+      </c>
+      <c r="E18">
+        <v>37.317</v>
+      </c>
+      <c r="F18">
+        <v>41</v>
+      </c>
+      <c r="G18">
+        <v>49</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="7">
+        <v>17.271429999999999</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19">
+        <v>34</v>
+      </c>
+      <c r="D19">
+        <v>38</v>
+      </c>
+      <c r="E19">
+        <v>43.582000000000001</v>
+      </c>
+      <c r="F19">
+        <v>48</v>
+      </c>
+      <c r="G19">
+        <v>55</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="7">
+        <v>16.533329999999999</v>
+      </c>
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20">
+        <v>36</v>
+      </c>
+      <c r="D20">
+        <v>40</v>
+      </c>
+      <c r="E20">
+        <v>46.881999999999998</v>
+      </c>
+      <c r="F20">
+        <v>52</v>
+      </c>
+      <c r="G20">
+        <v>59</v>
+      </c>
+      <c r="H20">
+        <v>1.02</v>
+      </c>
+      <c r="I20">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="7">
+        <v>14.16667</v>
+      </c>
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21">
+        <v>26</v>
+      </c>
+      <c r="D21">
+        <v>29</v>
+      </c>
+      <c r="E21">
+        <v>33.506</v>
+      </c>
+      <c r="F21">
+        <v>36</v>
+      </c>
+      <c r="G21">
+        <v>41</v>
+      </c>
+      <c r="H21">
+        <v>1.01</v>
+      </c>
+      <c r="I21">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="7">
+        <v>13.377780000000001</v>
+      </c>
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22">
+        <v>41</v>
+      </c>
+      <c r="D22">
+        <v>46</v>
+      </c>
+      <c r="E22">
+        <v>54.491</v>
+      </c>
+      <c r="F22">
+        <v>60</v>
+      </c>
+      <c r="G22">
+        <v>69</v>
+      </c>
+      <c r="H22">
+        <v>1.01</v>
+      </c>
+      <c r="I22">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="7">
+        <v>12.377780000000001</v>
+      </c>
+      <c r="B23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23">
+        <v>82</v>
+      </c>
+      <c r="D23">
+        <v>92</v>
+      </c>
+      <c r="E23">
+        <v>108.56100000000001</v>
+      </c>
+      <c r="F23">
+        <v>120</v>
+      </c>
+      <c r="G23">
+        <v>138</v>
+      </c>
+      <c r="H23">
+        <v>1.01</v>
+      </c>
+      <c r="I23">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="7">
+        <v>10.977779999999999</v>
+      </c>
+      <c r="B24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24">
+        <v>63</v>
+      </c>
+      <c r="D24">
+        <v>72</v>
+      </c>
+      <c r="E24">
+        <v>87.180999999999997</v>
+      </c>
+      <c r="F24">
+        <v>96</v>
+      </c>
+      <c r="G24">
+        <v>113</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="7">
+        <v>9.5444400000000016</v>
+      </c>
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25">
+        <v>47</v>
+      </c>
+      <c r="D25">
+        <v>54</v>
+      </c>
+      <c r="E25">
+        <v>63.844000000000001</v>
+      </c>
+      <c r="F25">
+        <v>71</v>
+      </c>
+      <c r="G25">
+        <v>81</v>
+      </c>
+      <c r="H25">
+        <v>1.05</v>
+      </c>
+      <c r="I25">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="7">
+        <v>7.4555600000000002</v>
+      </c>
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26">
+        <v>41</v>
+      </c>
+      <c r="D26">
+        <v>44</v>
+      </c>
+      <c r="E26">
+        <v>48.904000000000003</v>
+      </c>
+      <c r="F26">
+        <v>53</v>
+      </c>
+      <c r="G26">
+        <v>58</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="7">
+        <v>6.0888899999999992</v>
+      </c>
+      <c r="B27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27">
+        <v>56</v>
+      </c>
+      <c r="D27">
+        <v>62</v>
+      </c>
+      <c r="E27">
+        <v>71.052000000000007</v>
+      </c>
+      <c r="F27">
+        <v>78</v>
+      </c>
+      <c r="G27">
+        <v>89</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="7">
+        <v>5.0374999999999996</v>
+      </c>
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28">
+        <v>69</v>
+      </c>
+      <c r="D28">
+        <v>76</v>
+      </c>
+      <c r="E28">
+        <v>90.373999999999995</v>
+      </c>
+      <c r="F28">
+        <v>99</v>
+      </c>
+      <c r="G28">
+        <v>115</v>
+      </c>
+      <c r="H28">
+        <v>1.01</v>
+      </c>
+      <c r="I28">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="7">
+        <v>3.5777800000000006</v>
+      </c>
+      <c r="B29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29">
+        <v>36</v>
+      </c>
+      <c r="D29">
+        <v>40</v>
+      </c>
+      <c r="E29">
+        <v>47.795000000000002</v>
+      </c>
+      <c r="F29">
+        <v>52</v>
+      </c>
+      <c r="G29">
+        <v>61</v>
+      </c>
+      <c r="H29">
+        <v>1.01</v>
+      </c>
+      <c r="I29">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="7">
+        <v>2.9666700000000006</v>
+      </c>
+      <c r="B30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30">
+        <v>37</v>
+      </c>
+      <c r="D30">
+        <v>42</v>
+      </c>
+      <c r="E30">
+        <v>49.302999999999997</v>
+      </c>
+      <c r="F30">
+        <v>55</v>
+      </c>
+      <c r="G30">
+        <v>64</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="7">
+        <v>2.1888900000000007</v>
+      </c>
+      <c r="B31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31">
         <v>16</v>
       </c>
-      <c r="B10">
-        <v>102.09099999999999</v>
-      </c>
-      <c r="C10">
-        <v>105.446</v>
-      </c>
-      <c r="D10">
-        <v>118.60899999999999</v>
-      </c>
-      <c r="E10">
-        <v>116.86</v>
-      </c>
-      <c r="F10">
-        <v>168.03299999999999</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>32.970999999999997</v>
-      </c>
-      <c r="H10">
-        <v>1.0920000000000001</v>
-      </c>
-      <c r="I10">
-        <v>1.278</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <v>102.071</v>
-      </c>
-      <c r="C11">
-        <v>106.05200000000001</v>
-      </c>
-      <c r="D11">
-        <v>115.294</v>
-      </c>
-      <c r="E11">
-        <v>115.444</v>
-      </c>
-      <c r="F11">
-        <v>146.94399999999999</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>22.436499999999995</v>
-      </c>
-      <c r="H11">
-        <v>1.0489999999999999</v>
-      </c>
-      <c r="I11">
-        <v>1.1599999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="D31">
         <v>18</v>
       </c>
-      <c r="B12">
-        <v>113.053</v>
-      </c>
-      <c r="C12">
-        <v>116.78100000000001</v>
-      </c>
-      <c r="D12">
-        <v>127.32899999999999</v>
-      </c>
-      <c r="E12">
-        <v>127.968</v>
-      </c>
-      <c r="F12">
-        <v>158.34</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>22.643500000000003</v>
-      </c>
-      <c r="H12">
-        <v>1.0549999999999999</v>
-      </c>
-      <c r="I12">
-        <v>1.173</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13">
-        <v>122.837</v>
-      </c>
-      <c r="C13">
-        <v>126.636</v>
-      </c>
-      <c r="D13">
-        <v>134.023</v>
-      </c>
-      <c r="E13">
-        <v>137.126</v>
-      </c>
-      <c r="F13">
-        <v>150.52699999999999</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>13.844999999999992</v>
-      </c>
-      <c r="H13">
-        <v>1.0620000000000001</v>
-      </c>
-      <c r="I13">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14">
-        <v>108.982</v>
-      </c>
-      <c r="C14">
-        <v>114.77800000000001</v>
-      </c>
-      <c r="D14">
-        <v>126.596</v>
-      </c>
-      <c r="E14">
-        <v>124.898</v>
-      </c>
-      <c r="F14">
-        <v>177.524</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>34.271000000000001</v>
-      </c>
-      <c r="H14">
-        <v>1.105</v>
-      </c>
-      <c r="I14">
-        <v>1.32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15">
-        <v>104.32299999999999</v>
-      </c>
-      <c r="C15">
-        <v>109.992</v>
-      </c>
-      <c r="D15">
-        <v>117.438</v>
-      </c>
-      <c r="E15">
-        <v>120.005</v>
-      </c>
-      <c r="F15">
-        <v>141.16999999999999</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>18.423499999999997</v>
-      </c>
-      <c r="H15">
-        <v>1.1160000000000001</v>
-      </c>
-      <c r="I15">
-        <v>1.349</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16">
-        <v>84.188000000000002</v>
-      </c>
-      <c r="C16">
-        <v>90.388999999999996</v>
-      </c>
-      <c r="D16">
-        <v>97.234999999999999</v>
-      </c>
-      <c r="E16">
-        <v>99.706999999999994</v>
-      </c>
-      <c r="F16">
-        <v>115.485</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
-        <v>15.648499999999999</v>
-      </c>
-      <c r="H16">
-        <v>1.03</v>
-      </c>
-      <c r="I16">
-        <v>1.0940000000000001</v>
-      </c>
+      <c r="E31">
+        <v>21.477</v>
+      </c>
+      <c r="F31">
+        <v>24</v>
+      </c>
+      <c r="G31">
+        <v>28</v>
+      </c>
+      <c r="H31">
+        <v>1.01</v>
+      </c>
+      <c r="I31">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="7"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="7"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="7"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="7"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="7"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="7"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="7"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="7"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="7"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="7"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="7"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="7"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="7"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="7"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1697,34 +2294,34 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
-        <v>34</v>
-      </c>
       <c r="K1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L1" s="1">
         <v>0.85499999999999998</v>
@@ -1733,12 +2330,12 @@
         <v>1.2449899597988732E-2</v>
       </c>
       <c r="N1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>0.46800000000000003</v>
@@ -1759,7 +2356,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="K2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L2" s="1">
         <v>0.84029999999999994</v>
@@ -1768,12 +2365,12 @@
         <v>1.8814887722226777E-2</v>
       </c>
       <c r="N2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>0.15</v>
@@ -1804,7 +2401,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L4" s="4">
         <v>1.6953</v>
@@ -1813,7 +2410,7 @@
         <v>2.2561028345356952E-2</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -1826,765 +2423,765 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D203BF3-5E28-442F-8D97-BC84525A6BFD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02094578-3F68-4B90-BFBE-15CF3061CB4D}">
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="B2" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="C2" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="D2" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="E2" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F2" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="G2" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="H2" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="I2" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="J2" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="K2" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="L2" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="M2" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="N2" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="O2" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="B3" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="C3" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="D3" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="E3" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F3" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="G3" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="H3" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="I3" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="J3" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="K3" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="L3" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="M3" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="N3" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="O3" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="B4" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="C4" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="D4" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="E4" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F4" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="G4" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="H4" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="I4" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="J4" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="K4" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="L4" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="M4" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="N4" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="O4" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="B5" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="C5" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="D5" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="E5" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F5" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="G5" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="H5" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="I5" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="J5" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="K5" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="L5" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="M5" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="N5" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="O5" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="B6" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="C6" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="D6" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="E6" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="F6" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="G6" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="H6" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="I6" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="J6" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="K6" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="L6" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="M6" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="N6" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="O6" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="B7" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="C7" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="D7" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="E7" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F7" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="G7" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="H7" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="I7" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="J7" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="K7" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="L7" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="M7" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="N7" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="O7" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="B8" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="C8" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="D8" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="E8" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F8" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="G8" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="H8" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="I8" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="J8" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="K8" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="L8" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="M8" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="N8" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="O8" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="B9" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="C9" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="D9" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="E9" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F9" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="G9" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="H9" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="I9" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="J9" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="K9" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="L9" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="M9" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="N9" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="O9" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="B10" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="C10" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="D10" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="E10" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F10" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="G10" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="H10" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="I10" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="J10" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="K10" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="L10" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="M10" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="N10" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="O10" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="B11" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="C11" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="D11" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="E11" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F11" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="G11" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="H11" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="I11" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="J11" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="K11" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="L11" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="M11" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="N11" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="O11" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="B12" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="C12" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="D12" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="E12" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F12" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="G12" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="H12" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="I12" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="J12" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="K12" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="L12" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="M12" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="N12" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="O12" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="B13" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="C13" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="D13" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="E13" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F13" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="G13" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="H13" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="I13" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="J13" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="K13" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="L13" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="M13" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="N13" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="O13" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="B14" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="C14" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="D14" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="E14" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F14" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="G14" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="H14" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="I14" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="J14" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="K14" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="L14" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="M14" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="N14" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="O14" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="B15" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="C15" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="D15" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="E15" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F15" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="G15" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="H15" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="I15" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="J15" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="K15" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="L15" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="M15" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="N15" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="O15" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="B16" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="C16" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="D16" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="E16" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F16" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="G16" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="H16" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="I16" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="J16" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="K16" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="L16" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="M16" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="N16" s="2">
-        <v>2.0661479999999999E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="O16" s="2">
-        <v>6.7728399999999996E-3</v>
+        <v>5.9100000000000003E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2597,56 +3194,56 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>44</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>46</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>49</v>
-      </c>
-      <c r="O1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">

</xml_diff>